<commit_message>
tweak(template): move columns, add volume
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tommed/Desktop/scrape/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GitHub\epex-spot-scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9EB871-74BF-894D-A8A0-DC11ED99898D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5383E7-2FD4-4B94-BD13-54EFC05E6F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="900" windowWidth="28040" windowHeight="17180" xr2:uid="{440F71A1-88F8-4649-A567-7CE7E65AE17F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{440F71A1-88F8-4649-A567-7CE7E65AE17F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="EPEX Spot Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EPEX Spot Results'!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>HH</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Sell Volume</t>
+  </si>
+  <si>
+    <t>Volume</t>
   </si>
 </sst>
 </file>
@@ -453,50 +456,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A2A0E9-AD10-7648-97E1-74BE08DE37F9}">
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="4" width="15.69921875" style="1" customWidth="1"/>
+    <col min="5" max="8" width="22.69921875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:H1" xr:uid="{C3A2A0E9-AD10-7648-97E1-74BE08DE37F9}"/>
+  <autoFilter ref="A1:H1" xr:uid="{C3A2A0E9-AD10-7648-97E1-74BE08DE37F9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;R_x000D_&amp;1#&amp;"Aptos"&amp;10&amp;K000000 Internal Only</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(cron): run in arrears every night
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GitHub\epex-spot-scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5383E7-2FD4-4B94-BD13-54EFC05E6F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF803A9-2FA0-49E3-A403-7398F7B210DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{440F71A1-88F8-4649-A567-7CE7E65AE17F}"/>
   </bookViews>
@@ -69,7 +69,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,6 +92,13 @@
       <sz val="16"/>
       <color theme="0"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -115,15 +125,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,14 +472,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A2A0E9-AD10-7648-97E1-74BE08DE37F9}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="4" width="15.69921875" style="1" customWidth="1"/>
-    <col min="5" max="8" width="22.69921875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.69921875" style="1" customWidth="1"/>
+    <col min="6" max="8" width="22.69921875" style="4" customWidth="1"/>
     <col min="9" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
@@ -485,13 +498,13 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>